<commit_message>
added fastq file names back to 03.04.20
</commit_message>
<xml_diff>
--- a/fastqFiles/fastqFiles_03.04.20.xlsx
+++ b/fastqFiles/fastqFiles_03.04.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7922511-B4C4-0248-8914-D31F013FC61B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107A90E0-D7FD-3646-8C13-3EDCE243DCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27800" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="69">
   <si>
     <t>libraryDate</t>
   </si>
@@ -72,14 +72,173 @@
     <t>fullRNASeq</t>
   </si>
   <si>
-    <t>09.28.20</t>
+    <t>02.20.20</t>
+  </si>
+  <si>
+    <t>02.25.20</t>
+  </si>
+  <si>
+    <t>Brent_6a-1_GTAC1_SIC_Index2_07_TGAGGTT_GAGTTGGT_S2_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-2_GTAC2_SIC_Index2_07_GCTTAGA_GAGTTGGT_S3_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-3_GTAC3_SIC_Index2_07_ATGACAG_GAGTTGGT_S4_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-4_GTAC4_SIC_Index2_07_CACCTCC_GAGTTGGT_S5_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-5_GTAC5_SIC_Index2_07_ATCGAGC_GAGTTGGT_S6_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-6_GTAC6_SIC_Index2_07_TACTCTA_GAGTTGGT_S7_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-7_GTAC7_SIC_Index2_07_AGACTGA_GAGTTGGT_S8_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-8_GTAC8_SIC_Index2_07_CTTGGAA_GAGTTGGT_S9_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-9_GTAC9_SIC_Index2_07_CCGATTA_GAGTTGGT_S10_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-10_GTAC10_SIC_Index2_07_GGCAGCG_GAGTTGGT_S11_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-11_GTAC11_SIC_Index2_07_CCATCAT_GAGTTGGT_S12_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-12_GTAC12_SIC_Index2_07_TAACAAG_GAGTTGGT_S13_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-13_GTAC13_SIC_Index2_07_GAGGCGT_GAGTTGGT_S14_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-14_GTAC14_SIC_Index2_07_TTTAACT_GAGTTGGT_S15_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-15_GTAC15_SIC_Index2_07_GGTCCTC_GAGTTGGT_S16_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-16_GTAC16_SIC_Index2_07_CGGTGGC_GAGTTGGT_S17_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-17_GTAC17_SIC_Index2_07_ACTGTCG_GAGTTGGT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-18_GTAC18_SIC_Index2_07_GTATTTG_GAGTTGGT_S19_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-19_GTAC19_SIC_Index2_07_GAGTACG_GAGTTGGT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-20_GTAC20_SIC_Index2_07_ACAGATA_GAGTTGGT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-21_GTAC21_SIC_Index2_07_CTCAATG_GAGTTGGT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-22_GTAC22_SIC_Index2_07_AAATGCA_GAGTTGGT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-23_GTAC23_SIC_Index2_07_ACGCGGG_GAGTTGGT_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-24_GTAC24_SIC_Index2_07_GGAGTCC_GAGTTGGT_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-25_GTAC25_SIC_Index2_07_CGTCGCT_GAGTTGGT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6a-26_GTAC26_SIC_Index2_07_TCAACTG_GAGTTGGT_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-1_GTAC1_SIC_Index2_08_TGAGGTT_AAGCACGT_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-2_GTAC2_SIC_Index2_08_GCTTAGA_AAGCACGT_S29_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-3_GTAC3_SIC_Index2_08_ATGACAG_AAGCACGT_S30_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-4_GTAC4_SIC_Index2_08_CACCTCC_AAGCACGT_S31_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-5_GTAC5_SIC_Index2_08_ATCGAGC_AAGCACGT_S32_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-6_GTAC6_SIC_Index2_08_TACTCTA_AAGCACGT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-7_GTAC7_SIC_Index2_08_AGACTGA_AAGCACGT_S34_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-8_GTAC8_SIC_Index2_08_CTTGGAA_AAGCACGT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-9_GTAC9_SIC_Index2_08_CCGATTA_AAGCACGT_S36_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-10_GTAC10_SIC_Index2_08_GGCAGCG_AAGCACGT_S37_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-11_GTAC11_SIC_Index2_08_CCATCAT_AAGCACGT_S38_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-12_GTAC12_SIC_Index2_08_TAACAAG_AAGCACGT_S39_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-13_GTAC13_SIC_Index2_08_GAGGCGT_AAGCACGT_S40_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-14_GTAC14_SIC_Index2_08_TTTAACT_AAGCACGT_S41_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-15_GTAC15_SIC_Index2_08_GGTCCTC_AAGCACGT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-16_GTAC16_SIC_Index2_08_CGGTGGC_AAGCACGT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-17_GTAC17_SIC_Index2_08_ACTGTCG_AAGCACGT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-18_GTAC18_SIC_Index2_08_GTATTTG_AAGCACGT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-19_GTAC19_SIC_Index2_08_GAGTACG_AAGCACGT_S46_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-20_GTAC20_SIC_Index2_08_ACAGATA_AAGCACGT_S47_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-21_GTAC21_SIC_Index2_08_CTCAATG_AAGCACGT_S48_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-22_GTAC22_SIC_Index2_08_AAATGCA_AAGCACGT_S49_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-23_GTAC23_SIC_Index2_08_ACGCGGG_AAGCACGT_S50_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-24_GTAC24_SIC_Index2_08_GGAGTCC_AAGCACGT_S51_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-25_GTAC25_SIC_Index2_08_CGTCGCT_AAGCACGT_S52_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>Brent_6c-26_GTAC26_SIC_Index2_08_TCAACTG_AAGCACGT_S53_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,6 +251,12 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,11 +294,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,13 +616,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="9" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -499,7 +667,10 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -507,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -518,8 +689,17 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>7130292</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -527,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -538,8 +718,17 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>7465391</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -547,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -558,8 +747,17 @@
       <c r="G4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>6918095</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -567,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -578,8 +776,17 @@
       <c r="G5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>6938707</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -587,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -598,8 +805,17 @@
       <c r="G6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>7422430</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
@@ -607,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -618,8 +834,17 @@
       <c r="G7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>7328696</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -627,7 +852,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -638,8 +863,17 @@
       <c r="G8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>7124114</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -647,7 +881,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -658,8 +892,17 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>8048328</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -667,7 +910,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -678,8 +921,17 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>7263049</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -687,7 +939,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -698,8 +950,17 @@
       <c r="G11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>7789615</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -707,7 +968,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -718,8 +979,17 @@
       <c r="G12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>7374019</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -727,7 +997,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -738,8 +1008,17 @@
       <c r="G13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>7334606</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -747,7 +1026,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -758,8 +1037,17 @@
       <c r="G14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>7243273</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
@@ -767,7 +1055,7 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -778,8 +1066,17 @@
       <c r="G15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>7156193</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
@@ -787,7 +1084,7 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -798,8 +1095,17 @@
       <c r="G16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>7439127</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -807,7 +1113,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -818,8 +1124,17 @@
       <c r="G17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>6084413</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -827,7 +1142,7 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -838,8 +1153,17 @@
       <c r="G18" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>7635871</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -847,7 +1171,7 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -858,8 +1182,17 @@
       <c r="G19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>10748744</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -867,7 +1200,7 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -878,8 +1211,17 @@
       <c r="G20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>7404667</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -887,7 +1229,7 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -898,8 +1240,17 @@
       <c r="G21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>7237524</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -907,7 +1258,7 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -918,8 +1269,17 @@
       <c r="G22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>7328359</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -927,7 +1287,7 @@
         <v>22</v>
       </c>
       <c r="D23">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -938,8 +1298,17 @@
       <c r="G23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>7680303</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
@@ -947,7 +1316,7 @@
         <v>23</v>
       </c>
       <c r="D24">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -958,8 +1327,17 @@
       <c r="G24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>7433637</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -967,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -978,8 +1356,17 @@
       <c r="G25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>7749770</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -987,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="D26">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -998,8 +1385,17 @@
       <c r="G26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>7073397</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1403,7 @@
         <v>26</v>
       </c>
       <c r="D27">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1018,10 +1414,16 @@
       <c r="G27" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>7138988</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -1030,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -1041,10 +1443,16 @@
       <c r="G28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>9761671</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -1053,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -1064,10 +1472,16 @@
       <c r="G29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>7557623</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1076,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -1087,10 +1501,16 @@
       <c r="G30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>8579039</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1099,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1110,10 +1530,16 @@
       <c r="G31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>8379765</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1122,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="D32">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -1133,10 +1559,16 @@
       <c r="G32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>8717628</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -1145,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="D33">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -1156,10 +1588,16 @@
       <c r="G33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>7862673</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -1168,7 +1606,7 @@
         <v>7</v>
       </c>
       <c r="D34">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -1179,10 +1617,16 @@
       <c r="G34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>7690750</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -1191,7 +1635,7 @@
         <v>8</v>
       </c>
       <c r="D35">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -1202,10 +1646,16 @@
       <c r="G35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>9002102</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -1214,7 +1664,7 @@
         <v>9</v>
       </c>
       <c r="D36">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -1225,10 +1675,16 @@
       <c r="G36" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>7737452</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -1237,7 +1693,7 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -1248,10 +1704,16 @@
       <c r="G37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>6688367</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -1260,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="D38">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -1271,10 +1733,16 @@
       <c r="G38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>7160307</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -1283,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="D39">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -1294,10 +1762,16 @@
       <c r="G39" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>7412867</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -1306,7 +1780,7 @@
         <v>13</v>
       </c>
       <c r="D40">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1317,10 +1791,16 @@
       <c r="G40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>8347449</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -1329,7 +1809,7 @@
         <v>14</v>
       </c>
       <c r="D41">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -1340,10 +1820,16 @@
       <c r="G41" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>6819619</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -1352,7 +1838,7 @@
         <v>15</v>
       </c>
       <c r="D42">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1363,10 +1849,16 @@
       <c r="G42" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>17944222</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
@@ -1375,7 +1867,7 @@
         <v>16</v>
       </c>
       <c r="D43">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1386,10 +1878,16 @@
       <c r="G43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>9024416</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -1398,7 +1896,7 @@
         <v>17</v>
       </c>
       <c r="D44">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1409,10 +1907,16 @@
       <c r="G44" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>7875841</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
@@ -1421,7 +1925,7 @@
         <v>18</v>
       </c>
       <c r="D45">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1432,10 +1936,16 @@
       <c r="G45" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>7940535</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -1444,7 +1954,7 @@
         <v>19</v>
       </c>
       <c r="D46">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1455,10 +1965,16 @@
       <c r="G46" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>8577090</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -1467,7 +1983,7 @@
         <v>20</v>
       </c>
       <c r="D47">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1478,10 +1994,16 @@
       <c r="G47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>8870876</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -1490,7 +2012,7 @@
         <v>21</v>
       </c>
       <c r="D48">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1501,10 +2023,16 @@
       <c r="G48" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>7975280</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
@@ -1513,7 +2041,7 @@
         <v>22</v>
       </c>
       <c r="D49">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1524,10 +2052,16 @@
       <c r="G49" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>2170432</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -1536,7 +2070,7 @@
         <v>23</v>
       </c>
       <c r="D50">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -1547,10 +2081,16 @@
       <c r="G50" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>8990865</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -1559,7 +2099,7 @@
         <v>24</v>
       </c>
       <c r="D51">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -1570,10 +2110,16 @@
       <c r="G51" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>6238903</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -1582,7 +2128,7 @@
         <v>25</v>
       </c>
       <c r="D52">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -1593,10 +2139,16 @@
       <c r="G52" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>8335257</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -1605,7 +2157,7 @@
         <v>26</v>
       </c>
       <c r="D53">
-        <v>4621</v>
+        <v>4267</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -1615,6 +2167,12 @@
       </c>
       <c r="G53" t="s">
         <v>14</v>
+      </c>
+      <c r="J53">
+        <v>8520786</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>